<commit_message>
Fixed a logic mistake
</commit_message>
<xml_diff>
--- a/HW2/results.xlsx
+++ b/HW2/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\Desktop\W\4-1\CS454\HW\HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B35E3B-0D4F-40C8-98C8-EB5B24FD1035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97C083D-953C-4A71-B319-3A9D666FDFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7440" yWindow="555" windowWidth="21360" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nearest Mean" sheetId="1" r:id="rId1"/>
@@ -193,10 +193,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,24 +543,24 @@
     </row>
     <row r="6" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H6" s="7"/>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H7" s="7"/>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="5" t="s">
         <v>5</v>
       </c>
@@ -681,24 +681,24 @@
     </row>
     <row r="16" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H16" s="7"/>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H17" s="7"/>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J17" s="10"/>
+      <c r="J17" s="11"/>
       <c r="K17" s="5" t="s">
         <v>5</v>
       </c>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A3ADE0-344D-43B4-97DC-BCD7B01B5740}">
   <dimension ref="E4:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,25 +919,25 @@
     </row>
     <row r="8" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E8" s="7"/>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E9" s="7"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="6" t="s">
         <v>5</v>
       </c>
@@ -982,10 +982,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -1001,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J12" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -1067,25 +1067,25 @@
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E18" s="7"/>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E19" s="7"/>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="6" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I20" s="3">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <v>7</v>
       </c>
       <c r="H21" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I21" s="4">
         <v>20</v>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -1215,25 +1215,25 @@
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E28" s="8"/>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E29" s="8"/>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="10"/>
+      <c r="G29" s="11"/>
       <c r="H29" s="6" t="s">
         <v>5</v>
       </c>
@@ -1335,11 +1335,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="F29:G29"/>
     <mergeCell ref="F30:F32"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:J8"/>
@@ -1347,6 +1342,11 @@
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H18:J18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="F29:G29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>